<commit_message>
fixed feature file, fixed the old error, however new error where webdriverwait is not identifying the text is present, work on to fix it is in progress
</commit_message>
<xml_diff>
--- a/DaySix/CucumbExcel/src/test/resources/Data.xlsx
+++ b/DaySix/CucumbExcel/src/test/resources/Data.xlsx
@@ -8,15 +8,15 @@
     <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Credentials" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1708006262" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1708006262" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1708006262"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1708006262"/>
+      <pm:revision xmlns:pm="smNativeData" day="1708006357" val="1068" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1708006357" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1708006357" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1708006357"/>
     </ext>
   </extLst>
 </workbook>
@@ -37,14 +37,10 @@
     <t>https://rahulshettyacademy.com/client/</t>
   </si>
   <si>
-    <r>
-      <t>abcdef@abcd.com</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Abc12345</t>
-    </r>
+    <t>abcdef@abcd.com</t>
+  </si>
+  <si>
+    <t>Abc12345</t>
   </si>
 </sst>
 </file>
@@ -69,7 +65,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1708006262" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1708006357" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -84,7 +80,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1708006262" ulstyle="none">
+          <pm:charSpec xmlns:pm="smNativeData" id="1708006357" ulstyle="none">
             <pm:latin face="Consolas" sz="200" lang="default"/>
             <pm:cs face="Arial" sz="200" lang="default"/>
             <pm:ea face="Arial" sz="200" lang="default"/>
@@ -93,26 +89,15 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1708006262" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -128,26 +113,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1708006262"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1708006262"/>
+          <pm:border xmlns:pm="smNativeData" id="1708006357"/>
         </ext>
       </extLst>
     </border>
@@ -165,7 +131,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1708006262" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1708006357" count="1">
         <pm:charStyle name="Normal" fontId="0" Id="1"/>
       </pm:charStyles>
     </ext>
@@ -466,7 +432,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1708006262" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1708006357" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -475,16 +441,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1708006262" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1708006262" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1708006262" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1708006262" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1708006357" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1708006357" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1708006357" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1708006357" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1708006262" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1708006357" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>